<commit_message>
sync with jfic site
</commit_message>
<xml_diff>
--- a/docs/registration/jfic_supporter.xlsx
+++ b/docs/registration/jfic_supporter.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\22714789\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11160"/>
+    <workbookView xWindow="1080" yWindow="0" windowWidth="18080" windowHeight="8600"/>
   </bookViews>
   <sheets>
-    <sheet name="賛助会員登録申請" sheetId="2" r:id="rId1"/>
+    <sheet name="賛助会員登録申請（個人）" sheetId="2" r:id="rId1"/>
+    <sheet name="賛助会員申込（団体）" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,14 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>氏名</t>
-    <rPh sb="0" eb="2">
-      <t>シメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>（姓）</t>
     <rPh sb="1" eb="2">
@@ -198,107 +190,241 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2016年度　賛助会員登録申請</t>
-    <rPh sb="4" eb="6">
-      <t>ネンド</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>サンジョ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>カイイン</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>シンセイ</t>
+    <t>例</t>
+    <rPh sb="0" eb="1">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>送金先口座：
+連盟事務局：
+担当者：</t>
+    <rPh sb="0" eb="2">
+      <t>ソウキン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>コウザ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2016年   月   日</t>
+    <rPh sb="4" eb="5">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ガツ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ニチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>所在地</t>
+    <rPh sb="0" eb="3">
+      <t>sy</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>みずほ銀行　神戸支店　1550102　日本室内自転車競技連盟
+〒556-0014　大阪市浪速区大国3-9-15-601
+阪本博美　hiyoko_717@yahoo.co.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>団体・企業名</t>
+    <rPh sb="0" eb="6">
+      <t>ダンタ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <r>
-      <t>&lt;申請者通信欄&gt;　</t>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>○○</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>連盟</t>
+    </r>
+    <rPh sb="2" eb="4">
+      <t>レンメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>連盟　太郎</t>
+    <rPh sb="0" eb="2">
+      <t>レンメ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>タロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メールアドレス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>代表者名</t>
+    <rPh sb="0" eb="3">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ナマ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>団体を代表し、○○が○○○円を送金しました／します。</t>
+    <rPh sb="0" eb="2">
+      <t>ダンタ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ダイヒョウ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>エン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ソウキン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お名前</t>
+    <rPh sb="1" eb="3">
+      <t>ナマ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;申込者通信欄&gt;　</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
+        <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>※送金名と選手名が異なる場合は申請時にその旨をお知らせください</t>
+      <t>※送金される方とお申込者が異なる場合はお申込時にその旨をお知らせください</t>
     </r>
-    <rPh sb="1" eb="4">
+    <rPh sb="1" eb="3">
+      <t>モウシコm</t>
+    </rPh>
+    <rPh sb="3" eb="4">
       <t>シンセイシャ</t>
     </rPh>
     <rPh sb="4" eb="7">
       <t>ツウシンラン</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>例</t>
-    <rPh sb="0" eb="1">
-      <t>レイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>記載者全員を代表し、○○が合計○○○円を送金しました／します。</t>
-    <rPh sb="0" eb="3">
-      <t>キサイシャ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ゼンイン</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ダイヒョウ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ゴウケイ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
+    <rPh sb="15" eb="16">
+      <t>カt</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>シャ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>□□に代わり</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>、○○が○○○円を送金しました／します。</t>
+    </r>
+    <rPh sb="3" eb="4">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
       <t>エン</t>
     </rPh>
-    <rPh sb="20" eb="22">
+    <rPh sb="15" eb="17">
       <t>ソウキン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>送金先口座：
-連盟事務局：
-担当者：</t>
-    <rPh sb="0" eb="2">
-      <t>ソウキン</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>コウザ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>みずほ銀行　神戸支店　1550102　日本室内自転車競技連盟
-〒556-0014　大阪市浪速区大国3-9-15-601
-阪本博美</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2016年   月   日</t>
-    <rPh sb="4" eb="5">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ガツ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ニチ</t>
+    <t>2016年度　賛助会員申込（団体）</t>
+    <rPh sb="4" eb="6">
+      <t>ネンド</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>サンジョ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>カイイン</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>モウシコm</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ダン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2016年度　賛助会員申込（個人）</t>
+    <rPh sb="4" eb="6">
+      <t>ネンド</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>サンジョ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>カイイン</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>モウシコm</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>コジン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -307,7 +433,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,12 +517,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
+      <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="4">
@@ -419,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -429,42 +572,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -473,43 +616,170 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -561,6 +831,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -575,6 +858,10 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -596,10 +883,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -612,13 +911,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -634,6 +997,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>168165</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1338682" cy="822960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -670,76 +1082,11 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1338682" cy="822960"/>
+          <a:ext cx="1332332" cy="1000760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>715743</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>28573</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>288132</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>170436</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="図 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10897968" y="3829048"/>
-          <a:ext cx="1477389" cy="141863"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -790,7 +1137,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -825,7 +1172,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1002,7 +1349,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1010,251 +1357,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A6:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.75" style="4" customWidth="1"/>
-    <col min="4" max="5" width="15.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.83203125" style="4" customWidth="1"/>
+    <col min="4" max="5" width="12.5" style="4" customWidth="1"/>
     <col min="6" max="6" width="5.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="3.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20" style="4" customWidth="1"/>
-    <col min="13" max="14" width="25" style="4" customWidth="1"/>
-    <col min="15" max="15" width="7.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="4"/>
+    <col min="7" max="8" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="18" style="4" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25.83203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:15" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" s="2" customFormat="1" ht="20">
       <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="33"/>
-    </row>
-    <row r="7" spans="1:15" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="B7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-    </row>
-    <row r="9" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="25"/>
+    </row>
+    <row r="7" spans="1:15" s="3" customFormat="1" ht="32">
+      <c r="B7" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+    </row>
+    <row r="9" spans="1:15" ht="27" customHeight="1">
+      <c r="B9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="27" customHeight="1">
+      <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="N9" s="18" t="s">
+      <c r="C10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+    </row>
+    <row r="11" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-    </row>
-    <row r="11" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="D11" s="7">
         <v>2300001</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
       <c r="K11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N11" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>9</v>
       </c>
       <c r="O11" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="34" customHeight="1">
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B14" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-    </row>
-    <row r="16" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
+    <row r="13" spans="1:15" s="9" customFormat="1"/>
+    <row r="14" spans="1:15">
+      <c r="B14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+    </row>
+    <row r="16" spans="1:15" ht="27" customHeight="1">
+      <c r="B16" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="35"/>
       <c r="K16" s="10"/>
-      <c r="L16" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-    </row>
-    <row r="17" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L16" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+    </row>
+    <row r="17" spans="1:15" ht="27" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+        <v>20</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38"/>
       <c r="K17" s="11"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-    </row>
-    <row r="18" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+    </row>
+    <row r="18" spans="1:15" ht="27" customHeight="1">
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="12"/>
       <c r="N18" s="13"/>
     </row>
-    <row r="19" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+    <row r="19" spans="1:15" ht="27" customHeight="1">
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
       <c r="K19" s="14"/>
       <c r="L19" s="15"/>
       <c r="M19" s="13"/>
@@ -1300,7 +1649,315 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A6:P19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="4" customWidth="1"/>
+    <col min="5" max="6" width="12.83203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="29.1640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="20">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="25"/>
+    </row>
+    <row r="7" spans="1:16" s="3" customFormat="1" ht="32">
+      <c r="B7" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+    </row>
+    <row r="9" spans="1:16" ht="27" customHeight="1">
+      <c r="B9" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="49"/>
+      <c r="D9" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="27" customHeight="1">
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+    </row>
+    <row r="11" spans="1:16" s="6" customFormat="1" ht="27" customHeight="1">
+      <c r="A11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="53"/>
+      <c r="D11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="7">
+        <v>2300001</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="36" customHeight="1">
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" s="9" customFormat="1"/>
+    <row r="14" spans="1:16">
+      <c r="B14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+    </row>
+    <row r="16" spans="1:16" ht="29" customHeight="1">
+      <c r="B16" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+    </row>
+    <row r="17" spans="1:16" ht="27" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+    </row>
+    <row r="18" spans="1:16" ht="27" customHeight="1">
+      <c r="B18" s="42"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="13"/>
+    </row>
+    <row r="19" spans="1:16" ht="27" customHeight="1">
+      <c r="B19" s="45"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <mergeCells count="20">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="B14:O14"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="B7:O7"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B18:J19"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:N17"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12">
+      <formula1>"北海道,青森県,岩手県,宮城県,秋田県,山形県,福島県,茨城県,栃木県,群馬県,埼玉県,千葉県,東京都,神奈川県,新潟県,富山県,石川県,福井県,山梨県,長野県,岐阜県,静岡県,愛知県,三重県,滋賀県,京都府,大阪府,兵庫県,奈良県,和歌山県,鳥取県,島根県,岡山県,広島県,山口県,徳島県,香川県,愛媛県,高知県,福岡県,佐賀県,長崎県,熊本県,大分県,宮崎県,鹿児島県,沖縄県"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12">
+      <formula1>0</formula1>
+      <formula2>9999999</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O12">
+      <formula1>1</formula1>
+      <formula2>100000</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12">
+      <formula1>"する,しない"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>